<commit_message>
Add new versions of LIDO attribution qualifier clustering JSON and excel files
</commit_message>
<xml_diff>
--- a/DataValueClustering/experiments/exports/evaluation/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210319-133836.xlsx
+++ b/DataValueClustering/experiments/exports/evaluation/xlido_attribution_qualifier_randomized_0_1000000_hierarchical_20210319-133836.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viola Wenz\Documents\Repositories\data-value-clustering\DataValueClustering\experiments\exports\evaluation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster_Original" sheetId="1" r:id="rId1"/>
     <sheet name="Cluster_Repr" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -248,8 +253,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,7 +272,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFGREY"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -350,15 +355,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -400,7 +413,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,9 +445,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,6 +480,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -641,34 +656,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="50.7109375" customWidth="1"/>
     <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="50.7109375" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="50.7109375" customWidth="1"/>
     <col min="13" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="50.7109375" customWidth="1"/>
     <col min="17" max="17" width="6.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="50.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -705,7 +722,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,7 +763,7 @@
       </c>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
         <v>60</v>
       </c>
@@ -796,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J5" s="5" t="s">
         <v>53</v>
       </c>
@@ -816,7 +833,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J6" s="5" t="s">
         <v>54</v>
       </c>
@@ -836,7 +853,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J7" s="5" t="s">
         <v>55</v>
       </c>
@@ -856,7 +873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J8" s="5" t="s">
         <v>56</v>
       </c>
@@ -876,7 +893,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J9" s="5" t="s">
         <v>57</v>
       </c>
@@ -896,7 +913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L10" s="5" t="s">
         <v>11</v>
       </c>
@@ -910,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L11" s="5" t="s">
         <v>12</v>
       </c>
@@ -924,7 +941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L12" s="5" t="s">
         <v>13</v>
       </c>
@@ -938,7 +955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L13" s="5" t="s">
         <v>14</v>
       </c>
@@ -952,7 +969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L14" s="5" t="s">
         <v>15</v>
       </c>
@@ -966,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L15" s="5" t="s">
         <v>16</v>
       </c>
@@ -980,7 +997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L16" s="5" t="s">
         <v>17</v>
       </c>
@@ -994,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="12:15">
+    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L17" s="5" t="s">
         <v>18</v>
       </c>
@@ -1008,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="12:15">
+    <row r="18" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L18" s="5" t="s">
         <v>19</v>
       </c>
@@ -1022,7 +1039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="12:15">
+    <row r="19" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L19" s="5" t="s">
         <v>20</v>
       </c>
@@ -1036,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="12:15">
+    <row r="20" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L20" s="5" t="s">
         <v>21</v>
       </c>
@@ -1050,7 +1067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="12:15">
+    <row r="21" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L21" s="5" t="s">
         <v>22</v>
       </c>
@@ -1064,7 +1081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="12:15">
+    <row r="22" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L22" s="5" t="s">
         <v>23</v>
       </c>
@@ -1078,7 +1095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="12:15">
+    <row r="23" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L23" s="5" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="12:15">
+    <row r="24" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L24" s="5" t="s">
         <v>25</v>
       </c>
@@ -1106,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="12:15">
+    <row r="25" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N25" s="5" t="s">
         <v>48</v>
       </c>
@@ -1114,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="12:15">
+    <row r="26" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N26" s="5" t="s">
         <v>49</v>
       </c>
@@ -1122,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="12:15">
+    <row r="27" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N27" s="5" t="s">
         <v>50</v>
       </c>
@@ -1136,12 +1153,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1164,7 +1181,7 @@
     <col min="19" max="19" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1201,7 +1218,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
@@ -1242,7 +1259,7 @@
       </c>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1300,7 @@
       </c>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
         <v>60</v>
       </c>
@@ -1333,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J6" s="5" t="s">
         <v>53</v>
       </c>
@@ -1353,7 +1370,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J7" s="5" t="s">
         <v>55</v>
       </c>
@@ -1373,7 +1390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J8" s="5" t="s">
         <v>57</v>
       </c>
@@ -1393,7 +1410,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J9" s="5" t="s">
         <v>54</v>
       </c>
@@ -1413,7 +1430,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J10" s="5" t="s">
         <v>56</v>
       </c>
@@ -1433,7 +1450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1447,7 +1464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1461,7 +1478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1475,7 +1492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1489,7 +1506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1503,7 +1520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1517,7 +1534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="12:15">
+    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1531,7 +1548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="12:15">
+    <row r="18" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1545,7 +1562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="12:15">
+    <row r="19" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1559,7 +1576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="12:15">
+    <row r="20" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1573,7 +1590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="12:15">
+    <row r="21" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1587,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="12:15">
+    <row r="22" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L22" s="5" t="s">
         <v>25</v>
       </c>
@@ -1601,7 +1618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="12:15">
+    <row r="23" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N23" s="5" t="s">
         <v>48</v>
       </c>
@@ -1609,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="12:15">
+    <row r="24" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N24" s="5" t="s">
         <v>46</v>
       </c>
@@ -1617,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="12:15">
+    <row r="25" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1625,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="12:15">
+    <row r="26" spans="12:15" x14ac:dyDescent="0.25">
       <c r="N26" s="5" t="s">
         <v>49</v>
       </c>

</xml_diff>